<commit_message>
getting rid of them?
</commit_message>
<xml_diff>
--- a/data/survival/Westcott/B_survival_07172024.xlsx
+++ b/data/survival/Westcott/B_survival_07172024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceleuchtenberger/Library/Mobile Documents/com~apple~CloudDocs/Documents/project-gigas-conditioning-GL/data/survival/Westcott/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{053405B8-5288-A940-B612-B5D4310BC464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA89C34B-7BF3-3541-845C-E0A54085652A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6060" yWindow="1400" windowWidth="28040" windowHeight="17440" xr2:uid="{CA941532-24D2-184F-8B30-D5633C401736}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="31">
   <si>
     <t>bag_num</t>
   </si>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCF0E53-B26D-5F4D-A696-5BB849B2395F}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1563,6 +1563,9 @@
       <c r="F32" s="1">
         <v>45490</v>
       </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
       <c r="H32">
         <v>1</v>
       </c>
@@ -1592,6 +1595,9 @@
       <c r="F33" s="1">
         <v>45490</v>
       </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
       <c r="H33">
         <v>2</v>
       </c>
@@ -1621,6 +1627,9 @@
       <c r="F34" s="1">
         <v>45490</v>
       </c>
+      <c r="G34" t="s">
+        <v>10</v>
+      </c>
       <c r="H34">
         <v>3</v>
       </c>
@@ -1650,6 +1659,9 @@
       <c r="F35" s="1">
         <v>45490</v>
       </c>
+      <c r="G35" t="s">
+        <v>10</v>
+      </c>
       <c r="H35">
         <v>4</v>
       </c>
@@ -1679,6 +1691,9 @@
       <c r="F36" s="1">
         <v>45490</v>
       </c>
+      <c r="G36" t="s">
+        <v>10</v>
+      </c>
       <c r="H36">
         <v>5</v>
       </c>
@@ -1708,6 +1723,9 @@
       <c r="F37" s="1">
         <v>45490</v>
       </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
       <c r="H37">
         <v>6</v>
       </c>
@@ -1737,6 +1755,9 @@
       <c r="F38" s="1">
         <v>45490</v>
       </c>
+      <c r="G38" t="s">
+        <v>11</v>
+      </c>
       <c r="H38">
         <v>7</v>
       </c>
@@ -1766,6 +1787,9 @@
       <c r="F39" s="1">
         <v>45490</v>
       </c>
+      <c r="G39" t="s">
+        <v>10</v>
+      </c>
       <c r="H39">
         <v>8</v>
       </c>
@@ -1795,6 +1819,9 @@
       <c r="F40" s="1">
         <v>45490</v>
       </c>
+      <c r="G40" t="s">
+        <v>10</v>
+      </c>
       <c r="H40">
         <v>9</v>
       </c>
@@ -1823,6 +1850,9 @@
       </c>
       <c r="F41" s="1">
         <v>45490</v>
+      </c>
+      <c r="G41" t="s">
+        <v>10</v>
       </c>
       <c r="H41">
         <v>10</v>

</xml_diff>